<commit_message>
Attemp to get company for Indeed
</commit_message>
<xml_diff>
--- a/Multi_Indeed/job_data.xlsx
+++ b/Multi_Indeed/job_data.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IT Support Specialist I</t>
+          <t>IT Specialist (Remote)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,19 +488,19 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>$50,000 - $60,000 a year</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Compensation Range: $50,000 - $60,000 per year dependent upon experience</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IT Coordinator</t>
+          <t>IT PROFESSIONAL 2</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Proficient with Google products and Android (i.e. Google Business Suite) | Proficient with Apple products and iOS | Proficient with Windows products and operating software | Experience with HTML, Wordpress, Squarespace, and Shopify | Highly developed hardware/software troubleshooting techniques | Ability to provide L2/L3 technical support | Willingness to work a flexible schedule, including nights and weekends, based on the needs of the business | Excellent communication and problem solving skills</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -520,19 +520,19 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$55,000 - $65,000 a year</t>
+          <t>$73,310 - $109,641 a year</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Marketing &amp; Accounting Support</t>
+          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Product Support Specialist (Healthcare IT Support- Must have DICOM and HL7)</t>
+          <t>Supervisor, IT Service Desk</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -542,7 +542,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>401(k) | Dental insurance | Health insurance | Paid time off | Vision insurance</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -552,19 +552,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>$74,000 - $85,000 a year</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Travel:</t>
-        </is>
-      </c>
+          <t>$80,000 - $90,000 a year</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IT Specialist</t>
+          <t>IT Help Desk Technician</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -574,7 +570,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Manage user accounts. | Train new hires on infrastructure and operating system use. | Train users when systems or applications are upgraded. | Schedule requests to add, move or change hardware, software or phones. | Document procedures and maintain a library of information so that repeat questions or issues can be solved quickly</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -584,7 +580,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>$30.08 - $38.92 an hour</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -596,7 +592,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Help Desk Specialist</t>
+          <t>IT Service Desk Specialist</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -606,7 +602,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Maintain accurate logs of support requests, solutions, and follow-up actions in the help desk</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -624,7 +620,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Services Analyst - IT</t>
+          <t>IT Coordinator</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -634,7 +630,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Annual salary will vary based on a candidate's skills, qualifications, experience, and other factors: $84,000-$126,000 | Annual bonus and incentive pay up to 10% | 401(k) match and annual company contribution | Medical, Dental and Vision Insurance | Life and disability insurance | Generous paid time off, including vacation, floating and fixed holidays and sick time | Maternity leave as well as paid bonding/primary caregiver leave or parental leave for the birth or adoption of a child or to care for an ill family member, as applicable (eligibility based on position) | Long Term Incentive Plan for eligible positions | Wellbeing programs such as tuition reimbursement, adoption assistance and fitness reimbursement | Referral bonus program | And much more</t>
+          <t>Proficient with Google products and Android (i.e. Google Business Suite) | Proficient with Apple products and iOS | Proficient with Windows products and operating software | Experience with HTML, Wordpress, Squarespace, and Shopify | Highly developed hardware/software troubleshooting techniques | Ability to provide L2/L3 technical support | Willingness to work a flexible schedule, including nights and weekends, based on the needs of the business | Excellent communication and problem solving skills</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -644,19 +640,19 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$84,000 - $126,000 a year</t>
+          <t>$55,000 - $65,000 a year</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Marketing &amp; Accounting Support</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>IT Systems Administrator II – Denver International Airport</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -666,7 +662,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -676,19 +672,19 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$3,270 - $6,370 a month</t>
+          <t>$70,765 - $116,762 a year</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>The global Information Technology (IT) Function is leading efforts to align IT and Business Strategy, leverage IT investments, and optimize end to end business processes and associated information integration technologies. Through these efforts, IT helps to improve the competitive position of Corning's businesses through IT enabled processes. IT also delivers Information Technology applications, infrastructure, and project services in a cost efficient manner to Corning worldwide.</t>
+          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IT TECHNICIAN 4</t>
+          <t>Service Desk Technician - IT</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -708,19 +704,19 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>$56,689.00 - $83,666.16 a year</t>
+          <t>From $24.78 an hour</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Starting Hourly Rate: 24.78</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Service Desk Technician - IT</t>
+          <t>IT TECHNICIAN 4</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -740,19 +736,19 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>From $24.78 an hour</t>
+          <t>$56,689.00 - $83,666.16 a year</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Starting Hourly Rate: 24.78</t>
+          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IT Systems Administrator II – Denver International Airport</t>
+          <t>IT Support Specialist</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -762,7 +758,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -772,19 +768,15 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>$70,765 - $116,762 a year</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>IT Technician, Senior</t>
+          <t>IT Helpdesk Specialist</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -804,7 +796,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Day shift</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -816,7 +808,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>IT Customer Service Representative</t>
+          <t>Computer Systems Technician, Walt Disney World</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -836,7 +828,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>$37.43 an hour</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -848,7 +840,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IT Customer Support Paraprofessional</t>
+          <t>IT Specialist</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -858,7 +850,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Full-time schedule (12-months, 40-hours a week). | 6-month probationary period. | Criminal background check is required. | May be required to work alternate shift. | Requires local or regional travel. | On premise presence is required; 100% remote work is not available. | This position is designated a bargaining unit position. Membership is optional.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -868,19 +860,19 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>$3,999 - $5,370 a month</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>The Information Technology Division (IT) deploys strong technical skills and a passion for improving the lives of students, staff, and faculty in a dynamic teaching, learning, and working environment.</t>
+          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Desktop Technician - IT</t>
+          <t>Services Analyst - IT</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -890,7 +882,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Annual salary will vary based on a candidate's skills, qualifications, experience, and other factors: $84,000-$126,000 | Annual bonus and incentive pay up to 10% | 401(k) match and annual company contribution | Medical, Dental and Vision Insurance | Life and disability insurance | Generous paid time off, including vacation, floating and fixed holidays and sick time | Maternity leave as well as paid bonding/primary caregiver leave or parental leave for the birth or adoption of a child or to care for an ill family member, as applicable (eligibility based on position) | Long Term Incentive Plan for eligible positions | Wellbeing programs such as tuition reimbursement, adoption assistance and fitness reimbursement | Referral bonus program | And much more</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -900,19 +892,19 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>From $27.64 an hour</t>
+          <t>$84,000 - $126,000 a year</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Starting Hourly Rate: 27.64</t>
+          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IT Customer Support Representative</t>
+          <t>IT Support Technician 1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -932,7 +924,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>$20 - $27 an hour</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">

</xml_diff>

<commit_message>
Attemp to scrape multiple page
</commit_message>
<xml_diff>
--- a/Multi_Indeed/job_data.xlsx
+++ b/Multi_Indeed/job_data.xlsx
@@ -872,7 +872,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Services Analyst - IT</t>
+          <t>IT Support Technician 1</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Annual salary will vary based on a candidate's skills, qualifications, experience, and other factors: $84,000-$126,000 | Annual bonus and incentive pay up to 10% | 401(k) match and annual company contribution | Medical, Dental and Vision Insurance | Life and disability insurance | Generous paid time off, including vacation, floating and fixed holidays and sick time | Maternity leave as well as paid bonding/primary caregiver leave or parental leave for the birth or adoption of a child or to care for an ill family member, as applicable (eligibility based on position) | Long Term Incentive Plan for eligible positions | Wellbeing programs such as tuition reimbursement, adoption assistance and fitness reimbursement | Referral bonus program | And much more</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -892,7 +892,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>$84,000 - $126,000 a year</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IT Support Technician 1</t>
+          <t>IT Support Specialist Distribution Center</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -924,7 +924,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>$20.05 - $30.10 an hour</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">

</xml_diff>

<commit_message>
Data of all 5 pages
</commit_message>
<xml_diff>
--- a/Multi_Indeed/job_data.xlsx
+++ b/Multi_Indeed/job_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -592,7 +592,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT Service Desk Specialist</t>
+          <t>IT Coordinator</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -602,7 +602,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Proficient with Google products and Android (i.e. Google Business Suite) | Proficient with Apple products and iOS | Proficient with Windows products and operating software | Experience with HTML, Wordpress, Squarespace, and Shopify | Highly developed hardware/software troubleshooting techniques | Ability to provide L2/L3 technical support | Willingness to work a flexible schedule, including nights and weekends, based on the needs of the business | Excellent communication and problem solving skills</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -612,15 +612,19 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>$55,000 - $65,000 a year</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Marketing &amp; Accounting Support</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT Coordinator</t>
+          <t>IT Service Desk Specialist</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -630,7 +634,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Proficient with Google products and Android (i.e. Google Business Suite) | Proficient with Apple products and iOS | Proficient with Windows products and operating software | Experience with HTML, Wordpress, Squarespace, and Shopify | Highly developed hardware/software troubleshooting techniques | Ability to provide L2/L3 technical support | Willingness to work a flexible schedule, including nights and weekends, based on the needs of the business | Excellent communication and problem solving skills</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -640,19 +644,15 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$55,000 - $65,000 a year</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Marketing &amp; Accounting Support</t>
-        </is>
-      </c>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IT Events Program Manager</t>
+          <t>IT Systems Administrator II – Denver International Airport</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -672,15 +672,19 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$95,000 - $105,000 a year</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+          <t>$70,765 - $116,762 a year</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IT Systems Administrator II – Denver International Airport</t>
+          <t>IT TECHNICIAN 4</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -690,7 +694,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -700,7 +704,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>$70,765 - $116,762 a year</t>
+          <t>$56,689.00 - $83,666.16 a year</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -712,7 +716,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IT TECHNICIAN 4</t>
+          <t>Computer Systems Technician, Walt Disney World</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -732,7 +736,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>$56,689.00 - $83,666.16 a year</t>
+          <t>$37.43 an hour</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -808,7 +812,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Computer Systems Technician, Walt Disney World</t>
+          <t>Product Support Specialist (Healthcare IT Support- Must have DICOM and HL7)</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -818,7 +822,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>401(k) | Dental insurance | Health insurance | Paid time off | Vision insurance</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -828,19 +832,19 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>$37.43 an hour</t>
+          <t>$74,000 - $85,000 a year</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Travel:</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IT Support Technician 1</t>
+          <t>Services Analyst - IT</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -850,7 +854,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Annual salary will vary based on a candidate's skills, qualifications, experience, and other factors: $84,000-$126,000 | Annual bonus and incentive pay up to 10% | 401(k) match and annual company contribution | Medical, Dental and Vision Insurance | Life and disability insurance | Generous paid time off, including vacation, floating and fixed holidays and sick time | Maternity leave as well as paid bonding/primary caregiver leave or parental leave for the birth or adoption of a child or to care for an ill family member, as applicable (eligibility based on position) | Long Term Incentive Plan for eligible positions | Wellbeing programs such as tuition reimbursement, adoption assistance and fitness reimbursement | Referral bonus program | And much more</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -860,7 +864,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>$84,000 - $126,000 a year</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -900,7 +904,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IT Project Manager 1 (13351-2)</t>
+          <t>IT Support Technician 1</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -910,7 +914,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>$40</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -920,19 +924,19 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>$40 an hour</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Compensation</t>
+          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>IT Support Tier 1</t>
+          <t>IT Asset Coordinator</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -952,19 +956,19 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>No Location Available</t>
+          <t>$23.07 - $28.21 an hour</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>This job has no supervisory responsibilities.</t>
+          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IT Help Desk Technician</t>
+          <t>Computer Technician - 15452</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -974,7 +978,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Manage user accounts. | Train new hires on infrastructure and operating system use. | Train users when systems or applications are upgraded. | Schedule requests to add, move or change hardware, software or phones. | Document procedures and maintain a library of information so that repeat questions or issues can be solved quickly</t>
+          <t>Knowledge of healthcare regulations and compliance standards (e.g., HIPAA). | Understanding of data security and privacy practices in a healthcare setting.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -984,7 +988,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>$30.08 - $38.92 an hour</t>
+          <t>$23.76 - $36.82 an hour</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1028,7 +1032,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Computer Technician - 15452</t>
+          <t>Service Desk Analyst-Associate</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1038,7 +1042,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Knowledge of healthcare regulations and compliance standards (e.g., HIPAA). | Understanding of data security and privacy practices in a healthcare setting.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1048,7 +1052,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>$23.76 - $36.82 an hour</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1060,7 +1064,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IT Systems Administrator II – Denver International Airport</t>
+          <t>IT Support Technician 1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1070,7 +1074,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1080,7 +1084,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>$70,765 - $116,762 a year</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1092,7 +1096,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>IT Infrastructure Analyst (Alexandria, MN)</t>
+          <t>IT Support Tier 1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1112,19 +1116,19 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>$94,018 - $114,911 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>This job has no supervisory responsibilities.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IT Support Analyst, Rodeo Refinery</t>
+          <t>IT Technology Services Associate</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1144,19 +1148,19 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>$75,430 - $88,600 a year</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>We believe in the physical and mental well-being of our employees and are committed to offering comprehensive benefits that fit their personal needs. Our robust employee benefits package includes:</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Associate Tech User Support Analyst</t>
+          <t>Information Technology Specialist</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1176,19 +1180,19 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>$48,800 - $73,200 a year</t>
+          <t>$62,107 - $96,770 a year</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>This Direct-Hire position is in the Food and Drug Administration and is located in the Center for Tobacco Products (CTP), Office of Science (OS), Division of Regulatory Science Informatics (DRSI), Informatics Services and Support Branch. The Informatics Services and Support Branch is responsible for providing data and technology modernization, IT project management, customer service, and application learning/training support.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025 Early Talent – Technology - IT &amp; Cyber Risk</t>
+          <t>IT Support Specialist</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1198,7 +1202,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Medical | Health Advocate – This confidential service can help you; your spouse, dependent children, parents, and parents-in-law resolve health care and insurance-related issues, manage chronic conditions and improve your health and well-being. | Dental – Delta Dental PPO; DeltaCare USA | Vision – VSP Vision Plan | 401(k) | Flexible Spending Account | Onsite Wellness Clinic – Onsite physician for basic health and wellness consultations.</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1208,7 +1212,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>$60,000 - $92,000 a year</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1220,7 +1224,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Information Technology Specialist</t>
+          <t>IT Associate 1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1240,19 +1244,19 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>$62,107 - $96,770 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>This Direct-Hire position is in the Food and Drug Administration and is located in the Center for Tobacco Products (CTP), Office of Science (OS), Division of Regulatory Science Informatics (DRSI), Informatics Services and Support Branch. The Informatics Services and Support Branch is responsible for providing data and technology modernization, IT project management, customer service, and application learning/training support.</t>
+          <t>A maximum of 90 semester hours may be combined with experience or training in information technology to substitute for the baccalaureate degree.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>IT Support Analyst</t>
+          <t>IT Infrastructure Analyst (Alexandria, MN)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1272,7 +1276,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>No Location Available</t>
+          <t>$94,018 - $114,911 a year</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1284,7 +1288,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Associate IT Ops Specialist</t>
+          <t>IT Support Analyst</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1304,7 +1308,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>$56,200 - $92,800 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1316,7 +1320,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Analyst, Information Technology Support</t>
+          <t>IT Systems Administrator II – Denver International Airport</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1326,7 +1330,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1336,7 +1340,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>$70,765 - $116,762 a year</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1348,7 +1352,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>Computer Technician</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1368,7 +1372,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>$22.77 - $28.46 an hour</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1380,32 +1384,1468 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>Associate IT Ops Specialist</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>$56,200 - $92,800 a year</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Technology Support Technician</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>$55,265 - $61,406 a year</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>IT Support Analyst, Rodeo Refinery</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>$75,430 - $88,600 a year</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Information Technology Specialist</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>$62,107 - $96,770 a year</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>This Direct-Hire position is in the Food and Drug Administration and is located in the Center for Tobacco Products (CTP), Office of Science (OS), Division of Regulatory Science Informatics (DRSI), Informatics Services and Support Branch. The Informatics Services and Support Branch is responsible for providing data and technology modernization, IT project management, customer service, and application learning/training support.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>IT Systems Administrator I – Denver International Airport</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>$28.50 - $43.65 an hour</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Service Desk Technician, Tier I</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>$52,000 - $72,800 a year</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
           <t>Computer Technician</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>No Company Name Available</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Not Disclosed</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>$22.77 - $28.46 an hour</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>INFORMATION TECHNOLOGY ASSOCIATE</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>$4,791 - $8,485 a month</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>IT Systems Administrator II – Denver International Airport</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>$70,765 - $116,762 a year</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Computer Technician</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Public school</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>$46,000 - $52,000 a year</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>The information contained in this position description is in compliance with state and federal law (ADA, EEOC).</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>IT Support Specialist</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Service Desk Technician - IT</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>From $24.78 an hour</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Starting Hourly Rate: 24.78</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Information Technology Generalist I</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Your application must include aresume. | If you are claiming education in your answers to the supplemental application questions, you must attach a copy of your college transcripts for your claim to be accepted toward meeting the minimum requirements. Unofficial transcripts are acceptable. | Your application must be submitted by the posting closing date.Late applications and other required materials will not be accepted. | Failure to comply with the above application requirements may eliminate you from consideration for this position.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>$58,035 - $88,235 a year</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>IT SPECIALIST</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>This job operates in a professional office environment. This role routinely uses standard office equipment such as laptop computers, photocopiers, and smartphones.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>IT Technical Support Specialist</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>$60,774 - $87,515 a year</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>IT Specialist</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>IT Assistant</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Part-time</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>The mission of the Office of Student Financial Aid (OSFA) is to offer services and programs to students through awards funded from federal, state and private organizations. The primary mission of the Office is to provide eligible students with funds to finance and complete their education within the boundaries of federal, state and university regulations. The focus of the Office is to help students develop an understanding of the need to be proactive consumers of educational opportunities at George Mason University.</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>IT Security Analyst</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>$75,000 - $80,000 a year</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Pay Rate:Pay Range</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Information Systems Technician I</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>You will work on multiple assignments with competing deadlines | You will work in a busy, fast-paced workplace | Your customers will include some people with strong personalities and/or high expectations</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>$75,882.72 - $92,235.96 a year</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Information Technology (IT) Administrative Specialist</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Computer Technician</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Maintain a system log for the IVC classroom systems.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>$21.63 - $25.00 an hour</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Standard Hours per Week40</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Information Technology Trainee</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>$58,934.77 - $82,927.14 a year</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Help Desk Technician</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>$54,351.05 - $76,649.88 a year</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Experience:Minimum of 1 year of professional experience in providing technology support.</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>IT Support Technician</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>$58,500 - $62,000 a year</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Service Desk Analyst-Associate</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>RLF ASSOCIATE SERVICE DESK AGENT</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Know Me: Anticipate my needs and status to deliver effective care | Show Me the Way: Guide and prompt my actions to arrive at better outcomes and better health | Coordinate for Me: Own the complexity of my care through coordination</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>$27.36 - $34.90 an hour</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>These principles apply to ALL employees:SHC Commitment to Providing an Exceptional Patient &amp; Family ExperienceStanford Health Care sets a high standard for delivering value and an exceptional experience for our patients and families. Candidates for employment and existing employees must adopt and execute C-I-CARE standards for all of patients, families and towards each other. C-I-CARE is the foundation of Stanford’s patient-experience and represents a framework for patient-centered interactions. Simply put, we do what it takes to enable and empower patients and families to focus on health, healing and recovery.You will do this by executing against our three experience pillars, from the patient and family’s perspective:</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>IT Support Specialist</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Technology Experience Specialist Associate</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>$40,000 - $46,000 a year</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>To learn more about diversity, equity, and inclusion in LSA, please visit lsa.umich.edu/lsa/dei.</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>IT Support Specialist</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>About Us:Carroll College is a leading private, liberal arts college in the American West. Carroll’s campus rests on 63 acres at the edge of downtown and historic Helena, the capital city of Montana. The surrounding beauty of the Rocky Mountains and Montana fosters wonder and awe, giving the perfect backdrop to a worldly education. More than 75 miles of hiking and biking trails are just minutes from campus, and Helena is in close proximity to the Continental Divide Trail, natural hot springs, Great Divide Ski Area and the Missouri River. Yellowstone National Park and Glacier National Park are just a few hours away.</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>IT Associate</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Service Desk Specialist</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>High school graduate or equivalent; Associate or Bachelor’s degree in Information Technology or related field and/or industry recognized certifications are preferred | Obtain Support Analyst or Desktop Technician certification through the Help Desk Institute within approximately 1 year of hire | Valid driver's license and qualifying driving record for company automobile insurance</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>$25.58 - $34.70 an hour</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>IT Support Specialist</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>IT Support Analyst</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>IT Support Specialist Distribution Center</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>$20.05 - $30.10 an hour</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>IT Systems Administrator II – Denver International Airport</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>$70,765 - $116,762 a year</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>IT Help Desk Technician</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>This position is primarily performed in an indoor environment | While performing the duties of this job the employee is regularly required to: | Use hands to finger, handle, and feel | Sit, stand, walk, bend, and stoop | Sit at a desk or work center and operate a desktop or tablet computer, keyboard and mouse | Reach with hands and arms | Lift, carry, push and/or pull 10-20 lbs. | Talk and hear | While performing the duties of this job the employee is occasionally required to: | Crawl, climb, and crouch | Work in constrained spaces | Lift, carry, push and/or pull over 50 lbs. with assistance | Specific vision abilities required by this job include close vision, distance vision, color vision, and depth perception | There is minimal exposure to dust, dirt, and chemicals | The noise level in the work environment is generally moderate</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>CERTIFICATES, LICENSES AND REGISTRATIONS</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>IT Security Analyst</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>$75,000 - $80,000 a year</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Pay Rate:Pay Range</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>IT Help Desk Technician</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>$51,000 - $64,500 a year</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Education/Experience Guidelines:</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Service Desk Technician, Tier I</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>$52,000 - $72,800 a year</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Information Technology Analyst I</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>2024 “Great Place To Work Certified” | 2024 “America’s Best Large Employers” –Forbes | 2024 “Best Places to Work in IT” –Computerworld | 2023 “Best Employers for Women” –Forbes | 2023 “Workplace Well-being Platinum Winner” –Aetna | 2023 “America’s Best-In-State Employers” –Forbes | 2022 “LGBTQ+ Healthcare Equality Leader” - Human Rights Campaign | 2022 “Top 50 Companies for Diversity”– Diversity Inc. | 2022 “Best Company for Multicultural Women”– Seramount | 2022 “Top Company for Executive Women”- Seramount | “Silver HCM Excellence Award for Learning &amp; Development” –Brandon Hall Group | 2022 “Best Adoption Friendly Workplace” -Dave Thomas Foundation</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>$63,000 - $90,500 a year</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>NewYork-Presbyterian Hospital is an equal opportunity employer.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>IT Support Analyst I - IS Service Desk</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Behaves in a mindful manner focused on self, patient, visitor, and team safety. | Demonstrates accountability and commitment to quality work. | Participates actively in process improvement and adoption of standard work.</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>$21.36 - $26.70 an hour</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>IT Help Desk Technician (part-time)</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>$26 an hour</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>No Description Available</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Classroom Support Professional / Information Technology Professional</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>At-the-elbow customer service</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Information Technology Specialist (Non-Competitive)</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>$68,049.63 - $96,532.47 a year</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>CLOSING DATE:9/20/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>IT Support Specialist</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Full-time</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>IT Support Specialist</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>No Company Name Available</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>401(k) | 401(k) matching | Dental insurance | Vision insurance | Disability insurance | Health insurance | Health savings account | Life insurance | Paid time off | Floating holiday time | Mental health time off | Volunteer time off</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Not Disclosed</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>$54,000 - $68,000 a year</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Pay: $54,000 - $68,000 annually</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Indeed 5 page scrape
</commit_message>
<xml_diff>
--- a/Multi_Indeed/job_data.xlsx
+++ b/Multi_Indeed/job_data.xlsx
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Patriot Growth Insurance Services</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,12 +483,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$50,000 - $60,000 a year</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>$50,000 - $60,000 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -500,12 +500,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IT PROFESSIONAL 2</t>
+          <t>Supervisor, IT Service Desk</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Crocs</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -515,29 +515,25 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$80,000 - $90,000 a year</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$73,310 - $109,641 a year</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Supervisor, IT Service Desk</t>
+          <t>IT Service Desk Specialist</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Busey Bank</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -547,12 +543,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>$80,000 - $90,000 a year</t>
+          <t>14150 S Route 30, Plainfield, IL 60544</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -560,136 +556,140 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IT Help Desk Technician</t>
+          <t>IT Coordinator</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>RiverWILD</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Manage user accounts. | Train new hires on infrastructure and operating system use. | Train users when systems or applications are upgraded. | Schedule requests to add, move or change hardware, software or phones. | Document procedures and maintain a library of information so that repeat questions or issues can be solved quickly</t>
+          <t>Proficient with Google products and Android (i.e. Google Business Suite) | Proficient with Apple products and iOS | Proficient with Windows products and operating software | Experience with HTML, Wordpress, Squarespace, and Shopify | Highly developed hardware/software troubleshooting techniques | Ability to provide L2/L3 technical support | Willingness to work a flexible schedule, including nights and weekends, based on the needs of the business | Excellent communication and problem solving skills</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$55,000 - $65,000 a year</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>$30.08 - $38.92 an hour</t>
+          <t>114 West Main Street, Clayton, NC 27520</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Marketing &amp; Accounting Support</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IT Coordinator</t>
+          <t>IT Help Desk Technician</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>City of Plymouth, MN</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Proficient with Google products and Android (i.e. Google Business Suite) | Proficient with Apple products and iOS | Proficient with Windows products and operating software | Experience with HTML, Wordpress, Squarespace, and Shopify | Highly developed hardware/software troubleshooting techniques | Ability to provide L2/L3 technical support | Willingness to work a flexible schedule, including nights and weekends, based on the needs of the business | Excellent communication and problem solving skills</t>
+          <t>Manage user accounts. | Train new hires on infrastructure and operating system use. | Train users when systems or applications are upgraded. | Schedule requests to add, move or change hardware, software or phones. | Document procedures and maintain a library of information so that repeat questions or issues can be solved quickly</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$30.08 - $38.92 an hour</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>$55,000 - $65,000 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Marketing &amp; Accounting Support</t>
+          <t>$30.08 - $38.92 an hour</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IT Service Desk Specialist</t>
+          <t>IT Systems Administrator II – Denver International Airport</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>City and County of Denver</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$70,765 - $116,762 a year</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>$70,765 - $116,762 a year</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IT Systems Administrator II – Denver International Airport</t>
+          <t>Service Desk Technician - IT</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Hawaii Pacific Health</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>From $24.78 an hour</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$70,765 - $116,762 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Starting Hourly Rate: 24.78</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IT TECHNICIAN 4</t>
+          <t>Associate Tech User Support Analyst</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Medtronic</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -699,17 +699,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$48,800 - $73,200 a year</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>$56,689.00 - $83,666.16 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$48,800 - $73,200 a year</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Disney</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -731,29 +731,29 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$37.43 an hour</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>1050 Century Dr, Orlando, FL 32830</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>$37.43 an hour</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Associate Tech User Support Analyst</t>
+          <t>IT Specialist</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Refined Technologies</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -763,81 +763,77 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>$48,800 - $73,200 a year</t>
+          <t>480 Wildwood Forest Drive, Spring, TX 77380</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Full-time</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Information Technology Analyst I</t>
+          <t>IT Support Specialist</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Egnyte</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2024 “Great Place To Work Certified” | 2024 “America’s Best Large Employers” –Forbes | 2024 “Best Places to Work in IT” –Computerworld | 2023 “Best Employers for Women” –Forbes | 2023 “Workplace Well-being Platinum Winner” –Aetna | 2023 “America’s Best-In-State Employers” –Forbes | 2022 “LGBTQ+ Healthcare Equality Leader” - Human Rights Campaign | 2022 “Top 50 Companies for Diversity”– Diversity Inc. | 2022 “Best Company for Multicultural Women”– Seramount | 2022 “Top Company for Executive Women”- Seramount | “Silver HCM Excellence Award for Learning &amp; Development” –Brandon Hall Group | 2022 “Best Adoption Friendly Workplace” -Dave Thomas Foundation</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>$63,000 - $90,500 a year</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>NewYork-Presbyterian Hospital is an equal opportunity employer.</t>
-        </is>
-      </c>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Product Support Specialist (Healthcare IT Support- Must have DICOM and HL7)</t>
+          <t>IT TECHNICIAN 4</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>State of Nevada</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>401(k) | Dental insurance | Health insurance | Paid time off | Vision insurance</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$56,689.00 - $83,666.16 a year</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>$74,000 - $85,000 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Travel:</t>
+          <t>$56,689.00 - $83,666.16 a year</t>
         </is>
       </c>
     </row>
@@ -849,7 +845,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Exelon Corporation</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -859,29 +855,29 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$84,000 - $126,000 a year</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>$84,000 - $126,000 a year</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>IT SPECIALIST</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Volunteers of America Northern Rockies</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -891,25 +887,29 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr"/>
+          <t>1876 S Sheridan Ave, Sheridan, WY 82801</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>This job operates in a professional office environment. This role routinely uses standard office equipment such as laptop computers, photocopiers, and smartphones.</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>IT Support Technician 1</t>
+          <t>IT Helpdesk Specialist</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Tyler Technologies</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -924,24 +924,24 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Provide end-user support for Tyler’s internal customers via telephone, email, remote control and in-person. | Maintain a high level of courteous customer service at all times | Respond to emails, phone calls, and instant messages from Tyler employees requesting help with computer related issues | Learn the functions and back end of Tyler’s applications and corporate software so you can walk users through the steps to troubleshoot their issues or train them on processes | Aid the management team in conceptualizing updates and upgrades that will enhance Tyler’s employee’s experience</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>IT Asset Coordinator</t>
+          <t>IT Help Desk Technician</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Entech Engineering Inc</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -956,88 +956,84 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>$23.07 - $28.21 an hour</t>
+          <t>201 Penn Street, Reading, PA 19601</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Who we are:</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Computer Technician - 15452</t>
+          <t>Associate IT Ops Specialist</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>The Travelers Companies, Inc.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Knowledge of healthcare regulations and compliance standards (e.g., HIPAA). | Understanding of data security and privacy practices in a healthcare setting.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$56,200 - $92,800 a year</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>$23.76 - $36.82 an hour</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$56,200 - $92,800 a year</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>IT Technician 4</t>
+          <t>Help Desk Analyst 1</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>State of Georgia</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Utilize Oracle Customer Relationship Management (CRM) application to evaluate client’s comments including attachments, replies to typed responses to customer’s service request</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$38,452.58 - $50,142.29 a year</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Department: Continuous contact with departmental staff and student employees in support of client assistance regarding status and resolution of client issues.</t>
-        </is>
-      </c>
+          <t>200 Piedmont Ave SE # 1804, Atlanta, GA 30334</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Service Desk Analyst-Associate</t>
+          <t>Computer User Support Specialist 1, Digital Technology Solutions</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>University of Cincinnati</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1047,29 +1043,29 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$45,000 - $55,000 a year</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>For questions about the UC recruiting process or to request accommodations with the application, please contact Human Resources at jobs@uc.edu.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IT Support Technician 1</t>
+          <t>IT Support Analyst</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1084,24 +1080,24 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Provide technical support and consultation to internal users on matters relating to software, hardware, network, and mobile devices at multiple office locations. | Work as part of the Service Desk team to support and promote the goals of the organization.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>IT Support Tier 1</t>
+          <t>IT Support Technician</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Realign LLC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1111,7 +1107,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Contract</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1121,7 +1117,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>This job has no supervisory responsibilities.</t>
+          <t>Qualifications and Skills:</t>
         </is>
       </c>
     </row>
@@ -1133,7 +1129,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Mount Sinai Medical Center - Florida</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1143,12 +1139,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1160,12 +1156,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Information Technology Specialist</t>
+          <t>Technology Support Technician</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>University of North Carolina at Chapel Hill</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1175,61 +1171,61 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$55,265 - $61,406 a year</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>$62,107 - $96,770 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>This Direct-Hire position is in the Food and Drug Administration and is located in the Center for Tobacco Products (CTP), Office of Science (OS), Division of Regulatory Science Informatics (DRSI), Informatics Services and Support Branch. The Informatics Services and Support Branch is responsible for providing data and technology modernization, IT project management, customer service, and application learning/training support.</t>
+          <t>$55,265 - $61,406 a year</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>Computer Technician</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Whitehall-Coplay School District</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Medical | Health Advocate – This confidential service can help you; your spouse, dependent children, parents, and parents-in-law resolve health care and insurance-related issues, manage chronic conditions and improve your health and well-being. | Dental – Delta Dental PPO; DeltaCare USA | Vision – VSP Vision Plan | 401(k) | Flexible Spending Account | Onsite Wellness Clinic – Onsite physician for basic health and wellness consultations.</t>
+          <t>Public school</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$46,000 - $52,000 a year</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>$60,000 - $92,000 a year</t>
+          <t>2930 Zephyr Blvd, Whitehall Township, PA 18052</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>The information contained in this position description is in compliance with state and federal law (ADA, EEOC).</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IT Associate 1</t>
+          <t>IT Support Tier 1</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Meitheal Pharmaceuticals Inc</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1249,51 +1245,47 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>A maximum of 90 semester hours may be combined with experience or training in information technology to substitute for the baccalaureate degree.</t>
+          <t>This job has no supervisory responsibilities.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>IT Infrastructure Analyst (Alexandria, MN)</t>
+          <t>Sr Support Technician (Remote)</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Collins Aerospace</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Medical, dental, and vision insurance. | Three weeks of vacation for newly hired employees. | Generous 401(k) plan that includes employer matching funds and separate. employer retirement contribution, including a Lifetime Income Strategy option. | Tuition reimbursement program. | Student Loan Repayment Program. | Life insurance and disability coverage. | Optional coverages you can buy pet insurance, home and auto insurance, additional life and accident insurance, critical illness insurance, group legal, ID theft protection. | Birth, adoption, parental leave benefits. | Ovia Health, fertility, and family planning. | Adoption Assistance. | Autism Benefit. | Employee Assistance Plan, including up to 10 free counseling sessions. | Healthy You Incentives, wellness rewards program. | Doctor on Demand, virtual doctor visits. | Bright Horizons, child, and elder care services. | Teladoc Medical Experts, second opinion program. | And more!</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$37,000 - $83,000 a year</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>$94,018 - $114,911 a year</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>IT Support Analyst</t>
+          <t>Computer Technician</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Yuma County, AZ</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1303,61 +1295,61 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$22.77 - $28.46 an hour</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>No Location Available</t>
+          <t>198 South Main Street, Yuma, AZ 85364</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$22.77 - $28.46 an hour</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>IT Systems Administrator II – Denver International Airport</t>
+          <t>INFORMATION TECHNOLOGY ASSOCIATE</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>State Air Resources Board</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$4,791 - $8,485 a month</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>$70,765 - $116,762 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$4,791 - $8,485 a month</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Computer Technician</t>
+          <t>Help Desk Technician</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>The College of New Jersey</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1367,29 +1359,29 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$54,351.05 - $76,649.88 a year</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>$22.77 - $28.46 an hour</t>
+          <t>2000 Pennington Road, Ewing, NJ 08628</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Experience:Minimum of 1 year of professional experience in providing technology support.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Associate IT Ops Specialist</t>
+          <t>IT Technical Support Specialist</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>City of Portsmouth</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1399,29 +1391,29 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$60,774 - $87,515 a year</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>$56,200 - $92,800 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$60,774 - $87,515 a year</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Technology Support Technician</t>
+          <t>Help Desk Technician</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>The College of New Jersey</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1431,29 +1423,29 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$54,351.05 - $76,649.88 a year</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>$55,265 - $61,406 a year</t>
+          <t>2000 Pennington Road, Ewing, NJ 08628</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Experience:Minimum of 1 year of professional experience in providing technology support.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>IT Support Analyst, Rodeo Refinery</t>
+          <t>Computer Technician</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Buckeye Union School District</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1463,29 +1455,29 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$32.53 - $35.87 an hour</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>$75,430 - $88,600 a year</t>
+          <t>5049 Robert J Mathews Parkway, El Dorado Hills, CA 95762</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$32.53 - $35.87 an hour</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Information Technology Specialist</t>
+          <t>Computer Technician</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Yuma County, AZ</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1495,61 +1487,61 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$22.77 - $28.46 an hour</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>$62,107 - $96,770 a year</t>
+          <t>198 South Main Street, Yuma, AZ 85364</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>This Direct-Hire position is in the Food and Drug Administration and is located in the Center for Tobacco Products (CTP), Office of Science (OS), Division of Regulatory Science Informatics (DRSI), Informatics Services and Support Branch. The Informatics Services and Support Branch is responsible for providing data and technology modernization, IT project management, customer service, and application learning/training support.</t>
+          <t>$22.77 - $28.46 an hour</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>IT Systems Administrator I – Denver International Airport</t>
+          <t>INFORMATION TECHNOLOGY ASSOCIATE</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>State Air Resources Board</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$4,791 - $8,485 a month</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>$28.50 - $43.65 an hour</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$4,791 - $8,485 a month</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Service Desk Technician, Tier I</t>
+          <t>IT Support Analyst</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Houston Texans</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1564,56 +1556,56 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>$52,000 - $72,800 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Provide technical support and consultation to internal users on matters relating to software, hardware, network, and mobile devices at multiple office locations. | Work as part of the Service Desk team to support and promote the goals of the organization.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Computer Technician</t>
+          <t>Service Desk Specialist</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Blue Cross and Blue Shield of Kansas</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>High school graduate or equivalent; Associate or Bachelor’s degree in Information Technology or related field and/or industry recognized certifications are preferred | Obtain Support Analyst or Desktop Technician certification through the Help Desk Institute within approximately 1 year of hire | Valid driver's license and qualifying driving record for company automobile insurance</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$25.58 - $34.70 an hour</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>$22.77 - $28.46 an hour</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$25.58 - $34.70 an hour</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>INFORMATION TECHNOLOGY ASSOCIATE</t>
+          <t>Information Technology Specialist (Non-Competitive)</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>State of New Jersey</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1623,93 +1615,89 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$62,164.36 - $88,009.21 a year</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>$4,791 - $8,485 a month</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Existing Vacancies:One (1)</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>IT Systems Administrator II – Denver International Airport</t>
+          <t>Help Desk Specialist</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>MarineXchange Software GmbH</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+          <t>Maintain accurate logs of support requests, solutions, and follow-up actions in the help desk</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>$70,765 - $116,762 a year</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Computer Technician</t>
+          <t>Jr. IT Support Specialist</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>First Bank - NJ</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Public school</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>From $40,000 a year</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>$46,000 - $52,000 a year</t>
+          <t>First Bank - NJ in Township of Hamilton, NJ 08690</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>The information contained in this position description is in compliance with state and federal law (ADA, EEOC).</t>
+          <t>6) Manages the daily operation of the Help Desk system and coordinates support ticket distribution and resolution.</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>Service Desk Technician - IT</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Hawaii Pacific Health</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1719,93 +1707,93 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>From $24.78 an hour</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Starting Hourly Rate: 24.78</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Service Desk Technician - IT</t>
+          <t>ClassTech Support Analyst</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>North Carolina State University</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Takes responsibility for all classroom technology in the employee’s assigned zone.Monitoring incidents in ServiceNow to respond to tech support requests promptly | Monitoring incidents in ServiceNow to respond to tech support requests promptly | Plans organizes, and prioritizes work for themselves and the work of the student employees assigned to their zone. | Proactively prepares a weekly report for management to identify challenges, successes, or improvements within the employees’ assigned zones to management.</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$61,800 a year</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>From $24.78 an hour</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Starting Hourly Rate: 24.78</t>
+          <t>$61,800 a year</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Information Technology Generalist I</t>
+          <t>Information Technology Analyst</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Clean Water Services</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Your application must include aresume. | If you are claiming education in your answers to the supplemental application questions, you must attach a copy of your college transcripts for your claim to be accepted toward meeting the minimum requirements. Unofficial transcripts are acceptable. | Your application must be submitted by the posting closing date.Late applications and other required materials will not be accepted. | Failure to comply with the above application requirements may eliminate you from consideration for this position.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$46.21 - $63.54 an hour</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>$58,035 - $88,235 a year</t>
+          <t>2550 SW Hillsboro Hwy, Hillsboro, OR 97123</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$46.21 - $63.54 an hour</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>IT SPECIALIST</t>
+          <t>IT Support Technician</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Dine Brands</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1815,24 +1803,24 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>From $23 an hour</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>This job operates in a professional office environment. This role routinely uses standard office equipment such as laptop computers, photocopiers, and smartphones.</t>
+          <t>From $23 an hour</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>IT Technical Support Specialist</t>
+          <t>I.T. Help Desk Specialist</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1847,29 +1835,29 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>$60,774 - $87,515 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Athena Health Care Systems, headquartered in Connecticut, has been a pioneer in delivering exceptional healthcare services since its establishment in 1984. Operating nursing homes across Connecticut, Massachusetts, and Rhode Island, Athena stands out as one of the premier and highly regarded providers of skilled nursing centers in Southern New England. Through our commitment to improving both the lives of our residents and the quality of our environments, we have transformed our managed facilities into thriving communities where residents enjoy an enhanced quality of life, and employees find a fulfilling and supportive work environment.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>IT Specialist</t>
+          <t>INFORMATION TECHNOLOGY ANALYST-PART TIME</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Hyatt Regency Orlando Airport</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1879,61 +1867,61 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Part-time</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Part-time</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>IT Assistant</t>
+          <t>Computer Technician - 15452</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>University Medical Center of Southern Nevada</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Knowledge of healthcare regulations and compliance standards (e.g., HIPAA). | Understanding of data security and privacy practices in a healthcare setting.</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$23.76 - $36.82 an hour</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Part-time</t>
+          <t>1800 West Charleston Boulevard, Las Vegas, NV 89102</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>The mission of the Office of Student Financial Aid (OSFA) is to offer services and programs to students through awards funded from federal, state and private organizations. The primary mission of the Office is to provide eligible students with funds to finance and complete their education within the boundaries of federal, state and university regulations. The focus of the Office is to help students develop an understanding of the need to be proactive consumers of educational opportunities at George Mason University.</t>
+          <t>$23.76 - $36.82 an hour</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>IT Security Analyst</t>
+          <t>IT Support Analyst, Rodeo Refinery</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Phillips 66</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1943,61 +1931,61 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$75,430 - $88,600 a year</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>$75,000 - $80,000 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Pay Rate:Pay Range</t>
+          <t>$75,430 - $88,600 a year</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Information Systems Technician I</t>
+          <t>IT Help Desk Technician</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Appalachian Electric Cooperative</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>You will work on multiple assignments with competing deadlines | You will work in a busy, fast-paced workplace | Your customers will include some people with strong personalities and/or high expectations</t>
+          <t>This position is primarily performed in an indoor environment | While performing the duties of this job the employee is regularly required to: | Use hands to finger, handle, and feel | Sit, stand, walk, bend, and stoop | Sit at a desk or work center and operate a desktop or tablet computer, keyboard and mouse | Reach with hands and arms | Lift, carry, push and/or pull 10-20 lbs. | Talk and hear | While performing the duties of this job the employee is occasionally required to: | Crawl, climb, and crouch | Work in constrained spaces | Lift, carry, push and/or pull over 50 lbs. with assistance | Specific vision abilities required by this job include close vision, distance vision, color vision, and depth perception | There is minimal exposure to dust, dirt, and chemicals | The noise level in the work environment is generally moderate</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>$75,882.72 - $92,235.96 a year</t>
+          <t>1109 Hill Drive, New Market, TN 37820</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>CERTIFICATES, LICENSES AND REGISTRATIONS</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Information Technology (IT) Administrative Specialist</t>
+          <t>INFORMATION TECHNOLOGY TECHNICIAN</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>City of Huntington Beach, CA</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2007,93 +1995,93 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$53,934.40 - $72,280.00 a year</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$53,934.40 - $72,280.00 a year</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Computer Technician</t>
+          <t>Help Desk Technician</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>The College of New Jersey</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Maintain a system log for the IVC classroom systems.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$54,351.05 - $76,649.88 a year</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>$21.63 - $25.00 an hour</t>
+          <t>2000 Pennington Road, Ewing, NJ 08628</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Standard Hours per Week40</t>
+          <t>Experience:Minimum of 1 year of professional experience in providing technology support.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Information Technology Trainee</t>
+          <t>Information Technology Generalist I</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Commonwealth of PA</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Your application must include aresume. | If you are claiming education in your answers to the supplemental application questions, you must attach a copy of your college transcripts for your claim to be accepted toward meeting the minimum requirements. Unofficial transcripts are acceptable. | Your application must be submitted by the posting closing date.Late applications and other required materials will not be accepted. | Failure to comply with the above application requirements may eliminate you from consideration for this position.</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$58,035 - $88,235 a year</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>$58,934.77 - $82,927.14 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$58,035 - $88,235 a year</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Help Desk Technician</t>
+          <t>IT Assistant</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>George Mason University</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2103,29 +2091,29 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Part-time</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>$54,351.05 - $76,649.88 a year</t>
+          <t>4400 University Dr, Fairfax, VA 22030</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Experience:Minimum of 1 year of professional experience in providing technology support.</t>
+          <t>The mission of the Office of Student Financial Aid (OSFA) is to offer services and programs to students through awards funded from federal, state and private organizations. The primary mission of the Office is to provide eligible students with funds to finance and complete their education within the boundaries of federal, state and university regulations. The focus of the Office is to help students develop an understanding of the need to be proactive consumers of educational opportunities at George Mason University.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>IT Support Technician</t>
+          <t>Associate IT Ops Specialist</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>The Travelers Companies, Inc.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2135,24 +2123,24 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$56,200 - $92,800 a year</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>$58,500 - $62,000 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$56,200 - $92,800 a year</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Service Desk Analyst-Associate</t>
+          <t>IT Technology</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2167,61 +2155,61 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
           <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>RLF ASSOCIATE SERVICE DESK AGENT</t>
+          <t>IT Support Specialist</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Know Me: Anticipate my needs and status to deliver effective care | Show Me the Way: Guide and prompt my actions to arrive at better outcomes and better health | Coordinate for Me: Own the complexity of my care through coordination</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Up to $65,000 a year</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>$27.36 - $34.90 an hour</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>These principles apply to ALL employees:SHC Commitment to Providing an Exceptional Patient &amp; Family ExperienceStanford Health Care sets a high standard for delivering value and an exceptional experience for our patients and families. Candidates for employment and existing employees must adopt and execute C-I-CARE standards for all of patients, families and towards each other. C-I-CARE is the foundation of Stanford’s patient-experience and represents a framework for patient-centered interactions. Simply put, we do what it takes to enable and empower patients and families to focus on health, healing and recovery.You will do this by executing against our three experience pillars, from the patient and family’s perspective:</t>
+          <t>Up to $65,000 a year</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>IT Support Technician</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Hofstra University</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2231,29 +2219,29 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$58,500 - $62,000 a year</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>205 Hofstra University, Hempstead, NY 11549</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$58,500 - $62,000 a year</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Technology Experience Specialist Associate</t>
+          <t>IT Support Specialist</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>BBB Industries, LLC</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2263,24 +2251,24 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>$40,000 - $46,000 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>To learn more about diversity, equity, and inclusion in LSA, please visit lsa.umich.edu/lsa/dei.</t>
+          <t>Full-time</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>IT Specialist (Systems Analysis)</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2295,7 +2283,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$103,473 - $155,357 a year</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2305,19 +2293,19 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>About Us:Carroll College is a leading private, liberal arts college in the American West. Carroll’s campus rests on 63 acres at the edge of downtown and historic Helena, the capital city of Montana. The surrounding beauty of the Rocky Mountains and Montana fosters wonder and awe, giving the perfect backdrop to a worldly education. More than 75 miles of hiking and biking trails are just minutes from campus, and Helena is in close proximity to the Continental Divide Trail, natural hot springs, Great Divide Ski Area and the Missouri River. Yellowstone National Park and Glacier National Park are just a few hours away.</t>
+          <t>$103,473 - $155,357 a year</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>IT Associate</t>
+          <t>IT Help Desk Technician</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Vaupell Industrial</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2327,7 +2315,7 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$51,000 - $64,500 a year</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -2337,51 +2325,51 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Education/Experience Guidelines:</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Service Desk Specialist</t>
+          <t>IT Technician</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Nestlé Purina Pet Care</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>High school graduate or equivalent; Associate or Bachelor’s degree in Information Technology or related field and/or industry recognized certifications are preferred | Obtain Support Analyst or Desktop Technician certification through the Help Desk Institute within approximately 1 year of hire | Valid driver's license and qualifying driving record for company automobile insurance</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$48,000 - $69,000 a year</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>$25.58 - $34.70 an hour</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$48,000 - $69,000 a year</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>IT Support Technician</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>City of Denison</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2391,61 +2379,61 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$42,598.93 - $62,058.59 a year</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$42,598.93 - $62,058.59 a year</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>IT Support Analyst</t>
+          <t>IT Support Specialist</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Simplicity Credit Union</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>401(k) | 401(k) matching | Dental insurance | Vision insurance | Disability insurance | Health insurance | Health savings account | Life insurance | Paid time off | Floating holiday time | Mental health time off | Volunteer time off</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$54,000 - $68,000 a year</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>No Location Available</t>
+          <t>222 East Upham Street, Marshfield, WI 54449</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>Pay: $54,000 - $68,000 annually</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>IT Support Specialist Distribution Center</t>
+          <t>Assistant Computer Technician</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Westford Public Schools</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2455,93 +2443,93 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$33,200 a year</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>$20.05 - $30.10 an hour</t>
+          <t>23 Depot Street, Westford, MA 01886</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$33,200 a year</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>IT Systems Administrator II – Denver International Airport</t>
+          <t>Associate IT Ops Specialist</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>The Travelers Companies, Inc.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>FBI Background Check: FBI criminal background check is required for all positions at Denver International Airport (DEN). Employees are also required to report any felony convictions and/or moving violations to maintain this clearance and be eligible for continued employment. By position, a pre-employment physical/drug test may be required. | Snow/Emergency Duties: Denver International Airport is a 24/7/365 team operation. If weather conditions warrant or an emergency crisis occurs, all DEN employees can be required to work extended hours and/or shifts.</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$56,200 - $92,800 a year</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>$70,765 - $116,762 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$56,200 - $92,800 a year</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>IT Help Desk Technician</t>
+          <t>IT TECHNICIAN I</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>McLennan County, Texas</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>This position is primarily performed in an indoor environment | While performing the duties of this job the employee is regularly required to: | Use hands to finger, handle, and feel | Sit, stand, walk, bend, and stoop | Sit at a desk or work center and operate a desktop or tablet computer, keyboard and mouse | Reach with hands and arms | Lift, carry, push and/or pull 10-20 lbs. | Talk and hear | While performing the duties of this job the employee is occasionally required to: | Crawl, climb, and crouch | Work in constrained spaces | Lift, carry, push and/or pull over 50 lbs. with assistance | Specific vision abilities required by this job include close vision, distance vision, color vision, and depth perception | There is minimal exposure to dust, dirt, and chemicals | The noise level in the work environment is generally moderate</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$21.50 - $26.02 an hour</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Full-time</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>CERTIFICATES, LICENSES AND REGISTRATIONS</t>
+          <t>$21.50 - $26.02 an hour</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>IT Security Analyst</t>
+          <t>Information Systems Technician I</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Contra Costa County Superior Court</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2551,29 +2539,29 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$69,058.08 - $88,137.50 a year</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>$75,000 - $80,000 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Pay Rate:Pay Range</t>
+          <t>$69,058.08 - $88,137.50 a year</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>IT Help Desk Technician</t>
+          <t>Technology Support Specialist (TSPEC) PC 2265 SY 24/25</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Manassas City Public Schools</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2583,24 +2571,24 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$36.93 - $63.78 an hour</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>$51,000 - $64,500 a year</t>
+          <t>8700 Centreville Rd # 400, Manassas, VA 20110</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Education/Experience Guidelines:</t>
+          <t>FLSA Status: Non-Exempt</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Service Desk Technician, Tier I</t>
+          <t>IT Specialist (Systems Analysis)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -2615,93 +2603,89 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$103,473 - $155,357 a year</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>$52,000 - $72,800 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>$103,473 - $155,357 a year</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Information Technology Analyst I</t>
+          <t>IT Support Analyst I</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Orange County, NC</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>2024 “Great Place To Work Certified” | 2024 “America’s Best Large Employers” –Forbes | 2024 “Best Places to Work in IT” –Computerworld | 2023 “Best Employers for Women” –Forbes | 2023 “Workplace Well-being Platinum Winner” –Aetna | 2023 “America’s Best-In-State Employers” –Forbes | 2022 “LGBTQ+ Healthcare Equality Leader” - Human Rights Campaign | 2022 “Top 50 Companies for Diversity”– Diversity Inc. | 2022 “Best Company for Multicultural Women”– Seramount | 2022 “Top Company for Executive Women”- Seramount | “Silver HCM Excellence Award for Learning &amp; Development” –Brandon Hall Group | 2022 “Best Adoption Friendly Workplace” -Dave Thomas Foundation</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$46,755 - $54,221 a year</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>$63,000 - $90,500 a year</t>
+          <t>131 West Margaret Lane, Hillsborough, NC 27278</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>NewYork-Presbyterian Hospital is an equal opportunity employer.</t>
+          <t>$46,755 - $54,221 a year</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>IT Support Analyst I - IS Service Desk</t>
+          <t>Help Desk Specialist</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>MarineXchange Software GmbH</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Behaves in a mindful manner focused on self, patient, visitor, and team safety. | Demonstrates accountability and commitment to quality work. | Participates actively in process improvement and adoption of standard work.</t>
+          <t>Maintain accurate logs of support requests, solutions, and follow-up actions in the help desk</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>$21.36 - $26.70 an hour</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>No Description Available</t>
-        </is>
-      </c>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>IT Help Desk Technician (part-time)</t>
+          <t>Information Technology Specialist</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>FDA Center for Tobacco Products</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2711,29 +2695,29 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$62,107 - $96,770 a year</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>$26 an hour</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>No Description Available</t>
+          <t>This Direct-Hire position is in the Food and Drug Administration and is located in the Center for Tobacco Products (CTP), Office of Science (OS), Division of Regulatory Science Informatics (DRSI), Informatics Services and Support Branch. The Informatics Services and Support Branch is responsible for providing data and technology modernization, IT project management, customer service, and application learning/training support.</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Classroom Support Professional / Information Technology Professional</t>
+          <t>IT Specialist</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Refined Technologies</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2743,29 +2727,29 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
+          <t>480 Wildwood Forest Drive, Spring, TX 77380</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
           <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>At-the-elbow customer service</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Information Technology Specialist (Non-Competitive)</t>
+          <t>IT Support Specialist</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Virginia Tech</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2775,24 +2759,24 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Up to $65,000 a year</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>$68,049.63 - $96,532.47 a year</t>
+          <t>No Location Available</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>CLOSING DATE:9/20/2024</t>
+          <t>Up to $65,000 a year</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>I.T. Help Desk Specialist</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2807,45 +2791,49 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>Full-time</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Full-time</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr"/>
+          <t>No Location Available</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Athena Health Care Systems, headquartered in Connecticut, has been a pioneer in delivering exceptional healthcare services since its establishment in 1984. Operating nursing homes across Connecticut, Massachusetts, and Rhode Island, Athena stands out as one of the premier and highly regarded providers of skilled nursing centers in Southern New England. Through our commitment to improving both the lives of our residents and the quality of our environments, we have transformed our managed facilities into thriving communities where residents enjoy an enhanced quality of life, and employees find a fulfilling and supportive work environment.</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>IT Support Specialist</t>
+          <t>IT Help Desk Technician (part-time)</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>No Company Name Available</t>
+          <t>Rutgers University</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>401(k) | 401(k) matching | Dental insurance | Vision insurance | Disability insurance | Health insurance | Health savings account | Life insurance | Paid time off | Floating holiday time | Mental health time off | Volunteer time off</t>
+          <t>Not Disclosed</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Not Disclosed</t>
+          <t>$26 an hour</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>$54,000 - $68,000 a year</t>
+          <t>57 US Highway 1, New Brunswick, NJ 08901</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Pay: $54,000 - $68,000 annually</t>
+          <t>$26 an hour</t>
         </is>
       </c>
     </row>

</xml_diff>